<commit_message>
+ master gedung selesai, + update database & penjelasan
</commit_message>
<xml_diff>
--- a/PenjelasanDB.xlsx
+++ b/PenjelasanDB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Surya Bumantara\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\magang_ubs\ubs_codeigniter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D9786D-95D5-4E11-BC8E-2160E2C20720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09206E9-D7E0-4A9A-B4BC-E363524F1702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5244A7D-3EF8-4AD7-92BD-9EDF92A2BC67}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
   <si>
     <t>NAMA ASET</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>&lt;&lt;Nama Gedungnya&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;No IMB&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -566,7 +569,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,7 +677,7 @@
         <v>36</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
+ master kendaraan selesai
</commit_message>
<xml_diff>
--- a/PenjelasanDB.xlsx
+++ b/PenjelasanDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\magang_ubs\ubs_codeigniter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09206E9-D7E0-4A9A-B4BC-E363524F1702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96EAC7E-B87E-4DD3-B900-63517E820D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5244A7D-3EF8-4AD7-92BD-9EDF92A2BC67}"/>
   </bookViews>
@@ -569,7 +569,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
+ add desain transaksi
</commit_message>
<xml_diff>
--- a/PenjelasanDB.xlsx
+++ b/PenjelasanDB.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\magang_ubs\ubs_codeigniter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D96EAC7E-B87E-4DD3-B900-63517E820D4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3A901B-F5F8-401F-A521-102526B76F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C5244A7D-3EF8-4AD7-92BD-9EDF92A2BC67}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>NAMA ASET</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>&lt;&lt;No IMB&gt;&gt;</t>
+  </si>
+  <si>
+    <t>&lt;&lt;jumlah penghuni&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +747,7 @@
         <v>33</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>15</v>

</xml_diff>